<commit_message>
Committing new jar and new tests
</commit_message>
<xml_diff>
--- a/resources/api_document/dev_api_doc.xlsx
+++ b/resources/api_document/dev_api_doc.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UnimaOs\IdeaProjects\Pearson_Prep\Pearson_Prep_API_Test_Automation\resources\api_document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osanda Deshan\IdeaProjects\MaxSoft-IntelliAPI\resources\api_document\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD9EB7D-E832-43C1-8F3C-B4BC0F58248B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TestData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="171">
   <si>
     <t>API_NAME</t>
   </si>
@@ -136,15 +138,6 @@
   "description": "#description",
   "name": "#name"
 }</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8090/api/categories</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8090/api/decks</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8090/api/decks/users</t>
   </si>
   <si>
     <t>Recommendation API in Aggregation Service</t>
@@ -201,9 +194,6 @@
 }</t>
   </si>
   <si>
-    <t>http://10.199.253.187:8090/api/store</t>
-  </si>
-  <si>
     <t>Search Expert Decks using Expert Deck Service</t>
   </si>
   <si>
@@ -275,9 +265,6 @@
   </si>
   <si>
     <t>Edit MCQ Type Question using Aggregation Service</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8090/api/sync</t>
   </si>
   <si>
     <t>Sync API</t>
@@ -583,60 +570,15 @@
     <t>PLA Get Content API</t>
   </si>
   <si>
-    <t>http://10.199.253.187:8085/api/aggregated_questions/text</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8085/api/decks</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8085/api/decks/users</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8085/api/questions</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8085/api/questions/copy</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8085/api/learninganalytics/recommendations</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8085/api/learninganalytics/activities</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8085/api/cards/cloud</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8085/api/store/purchase/decks</t>
-  </si>
-  <si>
-    <t>http://10.199.240.44:8085/api/feedback</t>
-  </si>
-  <si>
-    <t>http://10.199.240.44:8085/api/version</t>
-  </si>
-  <si>
-    <t>http://10.199.240.44:8085/api/decks/onbording/users</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8085/api/questions/count</t>
-  </si>
-  <si>
     <t>Create Expert Bundle</t>
   </si>
   <si>
-    <t>http://10.199.253.187:8090/api/bundle/expert</t>
-  </si>
-  <si>
     <t>Edit Expert Bundle</t>
   </si>
   <si>
     <t>Get Expert Bundle</t>
   </si>
   <si>
-    <t>http://10.199.253.187:8090/api/store/users</t>
-  </si>
-  <si>
     <t>Create SKU</t>
   </si>
   <si>
@@ -650,12 +592,6 @@
   </si>
   <si>
     <t>Delete SKU</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8090/api/store/sku</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8085/api/store/sku</t>
   </si>
   <si>
     <t>{
@@ -692,13 +628,7 @@
     <t>Get Expert Bundle using Aggregation Service</t>
   </si>
   <si>
-    <t>http://10.199.253.187:8085/api/store/users</t>
-  </si>
-  <si>
     <t>Load Decks of a Bundle</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8085/api/bundle/expert</t>
   </si>
   <si>
     <t>Get a Bundle</t>
@@ -753,12 +683,6 @@
   </si>
   <si>
     <t>File Upload</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8085/api/cards/file</t>
-  </si>
-  <si>
-    <t>Get OAuth Access Token from Refresh Token</t>
   </si>
   <si>
     <t>{
@@ -855,31 +779,13 @@
 ]</t>
   </si>
   <si>
-    <t>Get the default 9 decks using Aggregation Service</t>
-  </si>
-  <si>
     <t>Search Expert Decks using Aggregation Service</t>
   </si>
   <si>
-    <t>http://10.199.253.187:8085/api/store</t>
-  </si>
-  <si>
     <t>Get A Category in Aggregation Service</t>
   </si>
   <si>
     <t>Get All Categories in Aggregation Service</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8085/api/categories</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8085/api/users/userId/bundle/expert</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8075/api/questions</t>
-  </si>
-  <si>
-    <t>http://10.199.253.187:8075/api/aggregated_questions/images/upload</t>
   </si>
   <si>
     <t>{
@@ -969,11 +875,173 @@
   ]
 }</t>
   </si>
+  <si>
+    <t>Copy Decks using Question Service</t>
+  </si>
+  <si>
+    <t>Get Questions Count using Question Service</t>
+  </si>
+  <si>
+    <t>Get Questions using Question Service</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/aggregated_questions/text</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/decks</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/decks/users</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/questions</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/questions/copy</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/categories</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/learninganalytics/recommendations</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/learninganalytics/activities</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/store</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/cards/cloud</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/store/purchase/decks</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/questions/count</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/store/users</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/store/sku</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/users/userId/bundle/expert</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/bundle/expert</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/cards/file</t>
+  </si>
+  <si>
+    <t>http://deckservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/store</t>
+  </si>
+  <si>
+    <t>http://deckservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/decks</t>
+  </si>
+  <si>
+    <t>http://deckservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/decks/users</t>
+  </si>
+  <si>
+    <t>http://deckservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/categories</t>
+  </si>
+  <si>
+    <t>http://deckservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/sync</t>
+  </si>
+  <si>
+    <t>http://deckservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/bundle/expert</t>
+  </si>
+  <si>
+    <t>http://deckservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/store/users</t>
+  </si>
+  <si>
+    <t>http://deckservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/store/sku</t>
+  </si>
+  <si>
+    <t>http://questionservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/questions</t>
+  </si>
+  <si>
+    <t>http://questionservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/aggregated_questions/images/upload</t>
+  </si>
+  <si>
+    <t>http://questionservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/questions/copy</t>
+  </si>
+  <si>
+    <t>http://questionservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/questions/count</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/feedback</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/version</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/decks/onbording/users</t>
+  </si>
+  <si>
+    <t>Delete MCQ Type Question using Question Service</t>
+  </si>
+  <si>
+    <t>Get the default decks using Aggregation Service</t>
+  </si>
+  <si>
+    <t>Purchase Bundle</t>
+  </si>
+  <si>
+    <t>Get All Decks For A User</t>
+  </si>
+  <si>
+    <t>http://aggregationservice-pearson-prep-us1-dev.bite.pearsondev.tech/api/store/purchase/bundles</t>
+  </si>
+  <si>
+    <t>Purchase Validator API</t>
+  </si>
+  <si>
+    <t>https://www.googleapis.com/androidpublisher/v3/applications/com.pearsoned.smartflashcards/purchases/products/#skuid/tokens/#purchaseToken?access_token=#access_token</t>
+  </si>
+  <si>
+    <t>Get Student Availability</t>
+  </si>
+  <si>
+    <t>http://groupworkservice-pearson-gw-us1-dev.bite.pearsondev.tech/api/v1</t>
+  </si>
+  <si>
+    <t>{
+  "courseId": "#courseId",
+  "userIds": [
+    "#userId1" , 
+     "#userId2"
+  ]
+}</t>
+  </si>
+  <si>
+    <t>Get OAuth Access Token from Refresh Token</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>osanda12</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Password1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1052,7 +1120,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1075,12 +1143,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1194,6 +1275,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1224,7 +1310,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2412,11 +2498,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E82"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B71" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2438,7 +2524,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>3</v>
@@ -2446,10 +2532,10 @@
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
@@ -2491,10 +2577,10 @@
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C5" s="39" t="s">
         <v>8</v>
@@ -2504,40 +2590,40 @@
     </row>
     <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C7" s="39" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="39"/>
       <c r="E7" s="39" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>8</v>
@@ -2547,10 +2633,10 @@
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C9" s="39" t="s">
         <v>10</v>
@@ -2560,25 +2646,25 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="40" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="C10" s="40" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="40"/>
       <c r="E10" s="40" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C11" s="28" t="s">
         <v>5</v>
@@ -2588,32 +2674,32 @@
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="40"/>
       <c r="E12" s="40" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="39" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C13" s="39" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="39"/>
       <c r="E13" s="39" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2621,14 +2707,14 @@
         <v>11</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="C14" s="40" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="40"/>
       <c r="E14" s="40" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2636,7 +2722,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>8</v>
@@ -2649,7 +2735,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>8</v>
@@ -2662,7 +2748,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>10</v>
@@ -2675,14 +2761,14 @@
         <v>17</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="C18" s="40" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="40"/>
       <c r="E18" s="40" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2690,7 +2776,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>8</v>
@@ -2700,10 +2786,10 @@
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>19</v>
+        <v>119</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>97</v>
+        <v>149</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>5</v>
@@ -2712,220 +2798,220 @@
       <c r="E20" s="15"/>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="39"/>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="39" t="s">
+      <c r="B26" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="39"/>
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="18"/>
+      <c r="E29" s="20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="39"/>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="C23" s="39" t="s">
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+    </row>
+    <row r="32" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+    </row>
+    <row r="33" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C33" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="D33" s="16"/>
+      <c r="E33" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+    </row>
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C35" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="39"/>
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C26" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="C27" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="20" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-    </row>
-    <row r="31" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-    </row>
-    <row r="32" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-    </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-    </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="B35" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
-        <v>143</v>
+      <c r="A36" s="22" t="s">
+        <v>114</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="C36" s="22" t="s">
         <v>8</v>
@@ -2934,11 +3020,11 @@
       <c r="E36" s="22"/>
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
-        <v>22</v>
+      <c r="A37" s="15" t="s">
+        <v>115</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>31</v>
+        <v>127</v>
       </c>
       <c r="C37" s="22" t="s">
         <v>8</v>
@@ -2946,98 +3032,98 @@
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="18" t="s">
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B39" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="15"/>
+      <c r="E39" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="22"/>
+      <c r="E40" s="24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+    </row>
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="B42" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="15"/>
-      <c r="E38" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B39" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="22"/>
-      <c r="E39" s="24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-    </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="22" t="s">
+      <c r="D42" s="22"/>
+      <c r="E42" s="26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="18"/>
+      <c r="E43" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B41" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="C41" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="22"/>
-      <c r="E41" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="18"/>
-      <c r="E42" s="20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B43" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" s="22"/>
-      <c r="E43" s="27"/>
     </row>
     <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
-        <v>140</v>
+        <v>35</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C44" s="22" t="s">
         <v>8</v>
@@ -3046,192 +3132,192 @@
       <c r="E44" s="27"/>
     </row>
     <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B45" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="C45" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="22"/>
+      <c r="E45" s="27"/>
+    </row>
+    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="18"/>
+      <c r="E46" s="20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="22"/>
+      <c r="E47" s="31"/>
+    </row>
+    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="18"/>
+      <c r="E48" s="31"/>
+    </row>
+    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B45" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C45" s="18" t="s">
+      <c r="B49" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="22"/>
+      <c r="E49" s="31"/>
+    </row>
+    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C50" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D45" s="18"/>
-      <c r="E45" s="20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B46" s="41" t="s">
+      <c r="D50" s="31"/>
+      <c r="E50" s="20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C46" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D46" s="22"/>
-      <c r="E46" s="31"/>
-    </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B47" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C47" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" s="18"/>
-      <c r="E47" s="31"/>
-    </row>
-    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="B48" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="C48" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" s="22"/>
-      <c r="E48" s="31"/>
-    </row>
-    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="B49" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C49" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" s="31"/>
-      <c r="E49" s="20" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="B50" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C50" s="27" t="s">
+      <c r="B51" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="C51" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-    </row>
-    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="C51" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51" s="31"/>
-      <c r="E51" s="20" t="s">
-        <v>68</v>
-      </c>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
     </row>
     <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="31" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>101</v>
+        <v>131</v>
       </c>
       <c r="C52" s="31" t="s">
         <v>5</v>
       </c>
       <c r="D52" s="31"/>
-      <c r="E52" s="31"/>
+      <c r="E52" s="20" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="B53" s="36" t="s">
-        <v>76</v>
+      <c r="A53" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>132</v>
       </c>
       <c r="C53" s="31" t="s">
         <v>5</v>
       </c>
       <c r="D53" s="31"/>
-      <c r="E53" s="42" t="s">
-        <v>77</v>
-      </c>
+      <c r="E53" s="31"/>
     </row>
     <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="33" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B54" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="C54" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="31"/>
+      <c r="E54" s="42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B55" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="C55" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D54" s="33"/>
-      <c r="E54" s="31"/>
-    </row>
-    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="B55" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="C55" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="31"/>
-      <c r="E55" s="42" t="s">
-        <v>77</v>
-      </c>
+      <c r="D55" s="33"/>
+      <c r="E55" s="31"/>
     </row>
     <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="B56" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C56" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="C56" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D56" s="33"/>
+      <c r="D56" s="31"/>
       <c r="E56" s="42" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="B57" s="19" t="s">
-        <v>103</v>
+        <v>77</v>
+      </c>
+      <c r="B57" s="41" t="s">
+        <v>78</v>
       </c>
       <c r="C57" s="33" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D57" s="33"/>
-      <c r="E57" s="31"/>
+      <c r="E57" s="42" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="34" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="C58" s="33" t="s">
         <v>8</v>
@@ -3240,276 +3326,276 @@
       <c r="E58" s="31"/>
     </row>
     <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="B59" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C59" s="40" t="s">
+      <c r="A59" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="B59" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C59" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="33"/>
+      <c r="E59" s="31"/>
+    </row>
+    <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C60" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D59" s="40"/>
-      <c r="E59" s="40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="B60" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="C60" s="39" t="s">
+      <c r="D60" s="40"/>
+      <c r="E60" s="40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="B61" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C61" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="D60" s="39"/>
-      <c r="E60" s="39" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="C61" s="40" t="s">
+      <c r="D61" s="39"/>
+      <c r="E61" s="39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C62" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D61" s="40"/>
-      <c r="E61" s="40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="B62" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C62" s="39" t="s">
+      <c r="D62" s="40"/>
+      <c r="E62" s="40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B63" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C63" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="D62" s="39"/>
-      <c r="E62" s="39" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="C63" s="40" t="s">
+      <c r="D63" s="39"/>
+      <c r="E63" s="39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C64" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="D63" s="40"/>
-      <c r="E63" s="40"/>
-    </row>
-    <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="B64" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="C64" s="39" t="s">
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+    </row>
+    <row r="65" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C65" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="D64" s="39"/>
-      <c r="E64" s="38"/>
-    </row>
-    <row r="65" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="B65" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="C65" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="D65" s="39"/>
-      <c r="E65" s="42" t="s">
-        <v>130</v>
-      </c>
+      <c r="D65" s="40"/>
+      <c r="E65" s="40"/>
     </row>
     <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="B66" s="41" t="s">
-        <v>107</v>
+        <v>87</v>
+      </c>
+      <c r="B66" s="37" t="s">
+        <v>86</v>
       </c>
       <c r="C66" s="39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D66" s="39"/>
-      <c r="E66" s="42" t="s">
-        <v>130</v>
-      </c>
+      <c r="E66" s="38"/>
     </row>
     <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="39" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="B67" s="41" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="C67" s="39" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D67" s="39"/>
-      <c r="E67" s="40"/>
+      <c r="E67" s="42" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="B68" s="41" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="C68" s="39" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D68" s="39"/>
-      <c r="E68" s="40"/>
+      <c r="E68" s="42" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="39" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="B69" s="41" t="s">
-        <v>116</v>
+        <v>145</v>
       </c>
       <c r="C69" s="39" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D69" s="39"/>
-      <c r="E69" s="20" t="s">
-        <v>118</v>
-      </c>
+      <c r="E69" s="40"/>
     </row>
     <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="39" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B70" s="41" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="C70" s="39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D70" s="39"/>
-      <c r="E70" s="20" t="s">
-        <v>118</v>
-      </c>
+      <c r="E70" s="40"/>
     </row>
     <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="39" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="B71" s="41" t="s">
-        <v>116</v>
+        <v>146</v>
       </c>
       <c r="C71" s="39" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D71" s="39"/>
-      <c r="E71" s="20"/>
+      <c r="E71" s="20" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="39" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="B72" s="41" t="s">
-        <v>117</v>
+        <v>146</v>
       </c>
       <c r="C72" s="39" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D72" s="39"/>
-      <c r="E72" s="20"/>
+      <c r="E72" s="20" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="39" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="B73" s="41" t="s">
-        <v>116</v>
+        <v>146</v>
       </c>
       <c r="C73" s="39" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D73" s="39"/>
-      <c r="E73" s="31"/>
+      <c r="E73" s="20"/>
     </row>
     <row r="74" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="B74" s="19" t="s">
-        <v>120</v>
+        <v>94</v>
+      </c>
+      <c r="B74" s="41" t="s">
+        <v>135</v>
       </c>
       <c r="C74" s="39" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D74" s="39"/>
-      <c r="E74" s="20" t="s">
-        <v>121</v>
-      </c>
+      <c r="E74" s="20"/>
     </row>
     <row r="75" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="B75" s="19" t="s">
-        <v>145</v>
+        <v>95</v>
+      </c>
+      <c r="B75" s="41" t="s">
+        <v>146</v>
       </c>
       <c r="C75" s="39" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D75" s="39"/>
       <c r="E75" s="31"/>
     </row>
     <row r="76" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="39" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C76" s="39" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D76" s="39"/>
-      <c r="E76" s="31"/>
+      <c r="E76" s="20" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="C77" s="39" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D77" s="39"/>
       <c r="E77" s="31"/>
     </row>
     <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="39" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="B78" s="19" t="s">
-        <v>107</v>
+        <v>144</v>
       </c>
       <c r="C78" s="39" t="s">
         <v>8</v>
@@ -3519,134 +3605,293 @@
     </row>
     <row r="79" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="39" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="B79" s="19" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
       <c r="C79" s="39" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D79" s="39"/>
       <c r="E79" s="31"/>
     </row>
     <row r="80" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="39" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
       <c r="B80" s="19" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="C80" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="D80" s="31" t="s">
-        <v>133</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D80" s="39"/>
       <c r="E80" s="31"/>
     </row>
     <row r="81" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="39" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="B81" s="19" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C81" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="D81" s="31" t="s">
-        <v>133</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D81" s="39"/>
       <c r="E81" s="31"/>
     </row>
     <row r="82" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="B82" s="21" t="s">
-        <v>96</v>
+        <v>164</v>
+      </c>
+      <c r="B82" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="C82" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="E82" s="31"/>
+    </row>
+    <row r="83" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="B83" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C83" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="E83" s="31"/>
+    </row>
+    <row r="84" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="B84" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C84" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="D82" s="39"/>
-      <c r="E82" s="39" t="s">
-        <v>150</v>
+      <c r="D84" s="39"/>
+      <c r="E84" s="39" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="B85" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C85" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" s="39"/>
+      <c r="E85" s="31"/>
+    </row>
+    <row r="86" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="B86" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C86" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D86" s="31"/>
+      <c r="E86" s="31"/>
+    </row>
+    <row r="87" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="B87" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="C87" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D87" s="31"/>
+      <c r="E87" s="31"/>
+    </row>
+    <row r="88" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="B88" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C88" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" s="31"/>
+      <c r="E88" s="31"/>
+    </row>
+    <row r="89" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="B89" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="C89" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" s="31"/>
+      <c r="E89" s="31"/>
+    </row>
+    <row r="90" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="43" t="s">
+        <v>161</v>
+      </c>
+      <c r="B90" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="C90" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D90" s="43"/>
+      <c r="E90" s="45" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="http://10.199.253.187:8070/api/questions"/>
-    <hyperlink ref="B6" r:id="rId2" display="http://10.199.253.187:8070/api/questions"/>
-    <hyperlink ref="B7" r:id="rId3" display="http://10.199.253.187:8070/api/questions"/>
-    <hyperlink ref="B8" r:id="rId4" display="http://10.199.253.187:8070/api/questions"/>
-    <hyperlink ref="B9" r:id="rId5" display="http://10.199.253.187:8070/api/questions"/>
-    <hyperlink ref="B10" r:id="rId6"/>
-    <hyperlink ref="B11" r:id="rId7" display="http://10.199.253.187:8070/api/aggregated_questions/images/upload"/>
-    <hyperlink ref="B13" r:id="rId8" display="http://10.199.253.187:8070/api/questions"/>
-    <hyperlink ref="B14" r:id="rId9"/>
-    <hyperlink ref="B17" r:id="rId10"/>
-    <hyperlink ref="B15" r:id="rId11"/>
-    <hyperlink ref="B16" r:id="rId12"/>
-    <hyperlink ref="B18" r:id="rId13"/>
-    <hyperlink ref="B19" r:id="rId14"/>
-    <hyperlink ref="B20" r:id="rId15"/>
-    <hyperlink ref="B30:B33" r:id="rId16" display="http://10.98.199.63:8085/api/decks"/>
-    <hyperlink ref="B40" r:id="rId17"/>
-    <hyperlink ref="B33" r:id="rId18"/>
-    <hyperlink ref="B29:B32" r:id="rId19" display="http://10.98.199.63:8085/api/decks"/>
-    <hyperlink ref="B31" r:id="rId20"/>
-    <hyperlink ref="B41" r:id="rId21"/>
-    <hyperlink ref="B42" r:id="rId22"/>
-    <hyperlink ref="B39" r:id="rId23"/>
-    <hyperlink ref="B44" r:id="rId24"/>
-    <hyperlink ref="B28" r:id="rId25"/>
-    <hyperlink ref="B12" r:id="rId26" display="http://10.199.253.187:8070/api/questions"/>
-    <hyperlink ref="B21" r:id="rId27"/>
-    <hyperlink ref="B45" r:id="rId28"/>
-    <hyperlink ref="B46" r:id="rId29"/>
-    <hyperlink ref="B47" r:id="rId30"/>
-    <hyperlink ref="B48" r:id="rId31"/>
-    <hyperlink ref="B49" r:id="rId32"/>
-    <hyperlink ref="B50" r:id="rId33"/>
-    <hyperlink ref="B51" r:id="rId34"/>
-    <hyperlink ref="B52" r:id="rId35"/>
-    <hyperlink ref="B2" r:id="rId36"/>
-    <hyperlink ref="B54" r:id="rId37"/>
-    <hyperlink ref="B53" r:id="rId38"/>
-    <hyperlink ref="B55" r:id="rId39"/>
-    <hyperlink ref="B56" r:id="rId40"/>
-    <hyperlink ref="B57" r:id="rId41"/>
-    <hyperlink ref="B58" r:id="rId42"/>
-    <hyperlink ref="B60" r:id="rId43"/>
-    <hyperlink ref="B59" r:id="rId44"/>
-    <hyperlink ref="B62" r:id="rId45" display="http://10.199.253.187:8070/api/questions"/>
-    <hyperlink ref="B61" r:id="rId46" display="http://10.199.253.187:8070/api/questions"/>
-    <hyperlink ref="B63" r:id="rId47"/>
-    <hyperlink ref="B64" r:id="rId48"/>
-    <hyperlink ref="B66" r:id="rId49"/>
-    <hyperlink ref="B67" r:id="rId50"/>
-    <hyperlink ref="B65" r:id="rId51"/>
-    <hyperlink ref="B73" r:id="rId52"/>
-    <hyperlink ref="B72" r:id="rId53"/>
-    <hyperlink ref="B74" r:id="rId54"/>
-    <hyperlink ref="B68" r:id="rId55"/>
-    <hyperlink ref="B75" r:id="rId56"/>
-    <hyperlink ref="B76" r:id="rId57"/>
-    <hyperlink ref="B77" r:id="rId58"/>
-    <hyperlink ref="B78" r:id="rId59"/>
-    <hyperlink ref="B79" r:id="rId60"/>
-    <hyperlink ref="B80" r:id="rId61"/>
-    <hyperlink ref="B81" r:id="rId62"/>
-    <hyperlink ref="B43" r:id="rId63"/>
-    <hyperlink ref="B36" r:id="rId64"/>
-    <hyperlink ref="B35" r:id="rId65"/>
+    <hyperlink ref="B5" r:id="rId1" display="http://10.199.253.187:8070/api/questions" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId2" display="http://10.199.253.187:8070/api/questions" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B7" r:id="rId3" display="http://10.199.253.187:8070/api/questions" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B8" r:id="rId4" display="http://10.199.253.187:8070/api/questions" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B9" r:id="rId5" display="http://10.199.253.187:8070/api/questions" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B10" r:id="rId6" display="http://10.199.253.187:8085/api/aggregated_questions/text" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B11" r:id="rId7" display="http://10.199.253.187:8070/api/aggregated_questions/images/upload" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B13" r:id="rId8" display="http://10.199.253.187:8070/api/questions" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B14" r:id="rId9" display="http://10.199.253.187:8085/api/decks" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B17" r:id="rId10" display="http://10.199.253.187:8085/api/decks" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B15" r:id="rId11" display="http://10.199.253.187:8085/api/decks/users" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B16" r:id="rId12" display="http://10.199.253.187:8085/api/decks" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B18" r:id="rId13" display="http://10.199.253.187:8085/api/decks" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B19" r:id="rId14" display="http://10.199.253.187:8085/api/questions" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B21" r:id="rId15" display="http://10.199.253.187:8085/api/questions/copy" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B31:B34" r:id="rId16" display="http://10.98.199.63:8085/api/decks" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B41" r:id="rId17" display="http://10.199.253.187:8090/api/categories" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B34" r:id="rId18" display="http://10.199.253.187:8090/api/decks" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B30:B33" r:id="rId19" display="http://10.98.199.63:8085/api/decks" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B32" r:id="rId20" display="http://10.199.253.187:8090/api/decks/users" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B42" r:id="rId21" display="http://10.199.253.187:8085/api/learninganalytics/recommendations" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B43" r:id="rId22" display="http://10.199.253.187:8085/api/learninganalytics/activities" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B40" r:id="rId23" display="http://10.199.253.187:8090/api/categories" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B45" r:id="rId24" display="http://10.199.253.187:8085/api/store" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B29" r:id="rId25" display="http://10.199.253.187:8090/api/store" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B12" r:id="rId26" display="http://10.199.253.187:8070/api/questions" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B22" r:id="rId27" display="http://10.199.253.187:8085/api/questions" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B46" r:id="rId28" display="http://10.199.253.187:8090/api/sync" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B47" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B48" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B49" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B50" r:id="rId32" display="http://10.199.253.187:8090/api/store" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B51" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B52" r:id="rId34" display="http://10.199.253.187:8085/api/cards/cloud" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B53" r:id="rId35" display="http://10.199.253.187:8085/api/store/purchase/decks" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B2" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B55" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B54" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B56" r:id="rId39" display="http://10.199.240.44:8085/api/feedback" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B57" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B58" r:id="rId41" display="http://10.199.240.44:8085/api/version" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B59" r:id="rId42" display="http://10.199.240.44:8085/api/decks/onbording/users" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B61" r:id="rId43" display="http://10.199.253.187:8085/api/questions" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B60" r:id="rId44" display="http://10.199.253.187:8085/api/questions" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B63" r:id="rId45" display="http://10.199.253.187:8070/api/questions" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B62" r:id="rId46" display="http://10.199.253.187:8070/api/questions" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B65" r:id="rId47" display="http://10.199.253.187:8085/api/questions/count" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B66" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B68" r:id="rId49" display="http://10.199.253.187:8090/api/bundle/expert" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B69" r:id="rId50" display="http://10.199.253.187:8090/api/store/users" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B67" r:id="rId51" display="http://10.199.253.187:8090/api/bundle/expert" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B75" r:id="rId52" display="http://10.199.253.187:8090/api/store/sku" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B74" r:id="rId53" display="http://10.199.253.187:8085/api/store/sku" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B76" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B70" r:id="rId55" display="http://10.199.253.187:8085/api/store/users" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B77" r:id="rId56" display="http://10.199.253.187:8085/api/users/userId/bundle/expert" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B78" r:id="rId57" display="http://10.199.253.187:8090/api/bundle/expert" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B79" r:id="rId58" display="http://10.199.253.187:8090/api/bundle/expert" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B80" r:id="rId59" display="http://10.199.253.187:8090/api/bundle/expert" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B81" r:id="rId60" display="http://10.199.253.187:8085/api/bundle/expert" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B83" r:id="rId61" display="http://10.199.253.187:8085/api/cards/file" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B44" r:id="rId62" display="http://10.199.253.187:8090/api/store" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B37" r:id="rId63" display="http://10.199.253.187:8085/api/categories" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B36" r:id="rId64" display="http://10.199.253.187:8085/api/categories" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B20" r:id="rId65" display="http://10.199.253.187:8070/api/questions/copy" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B64" r:id="rId66" display="http://10.199.253.187:8070/api/questions/count" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B85" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B84" r:id="rId68" display="http://10.199.253.187:8085/api/questions" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B73" r:id="rId69" display="http://10.199.253.187:8090/api/store/sku" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B86" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B87" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B88" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B82" r:id="rId73" xr:uid="{15237614-B87C-4E4D-9423-45109FC23D23}"/>
+    <hyperlink ref="B89" r:id="rId74" location="skuid/tokens/#purchaseToken?access_token=#access_token" xr:uid="{BFE1CFF8-6989-458D-9405-C3F6C670AFE4}"/>
+    <hyperlink ref="B90" r:id="rId75" xr:uid="{539FF276-D786-409A-BF7A-187F12475439}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId66"/>
+  <pageSetup orientation="portrait" r:id="rId76"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B640F4-2680-42F8-9ABB-15C499068C76}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>